<commit_message>
Add version to antibodies.tsv
</commit_message>
<xml_diff>
--- a/docs/antibodies/antibodies.xlsx
+++ b/docs/antibodies/antibodies.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,11 +29,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Current version of metadata schema. Template provides the correct value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Structure of channel_id depends on assay type.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +142,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
   <si>
     <t>channel_id</t>
   </si>
@@ -500,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -509,34 +529,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add concentration to antibodies
</commit_message>
<xml_diff>
--- a/docs/antibodies/antibodies.xlsx
+++ b/docs/antibodies/antibodies.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
     <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="concentration_unit list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -120,11 +121,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>TODO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TODO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>An antibody may be conjugated to a fluorescent tag or a metal tag for detection. Conjugated antibodies may be purchased from commercial providers.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,12 +169,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>channel_id</t>
@@ -166,6 +193,15 @@
   </si>
   <si>
     <t>dilution</t>
+  </si>
+  <si>
+    <t>concentration_value</t>
+  </si>
+  <si>
+    <t>concentration_unit</t>
+  </si>
+  <si>
+    <t>ug/ml</t>
   </si>
   <si>
     <t>conjugated_cat_number</t>
@@ -520,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -529,7 +565,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,11 +593,24 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="H2:H1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ug/ml." sqref="I2:I1048576">
+      <formula1>'concentration_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -585,4 +634,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Add concentration to antibodies"
This reverts commit 96bd78ac380895e52ef5db940f88496b6d46734e.
</commit_message>
<xml_diff>
--- a/docs/antibodies/antibodies.xlsx
+++ b/docs/antibodies/antibodies.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
     <sheet name="version list" sheetId="2" r:id="rId2"/>
-    <sheet name="concentration_unit list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -121,37 +120,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>TODO</t>
+          <t>An antibody may be conjugated to a fluorescent tag or a metal tag for detection. Conjugated antibodies may be purchased from commercial providers.</t>
         </r>
       </text>
     </comment>
     <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>TODO</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>An antibody may be conjugated to a fluorescent tag or a metal tag for detection. Conjugated antibodies may be purchased from commercial providers.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,12 +142,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1</t>
   </si>
   <si>
     <t>channel_id</t>
@@ -193,15 +166,6 @@
   </si>
   <si>
     <t>dilution</t>
-  </si>
-  <si>
-    <t>concentration_value</t>
-  </si>
-  <si>
-    <t>concentration_unit</t>
-  </si>
-  <si>
-    <t>ug/ml</t>
   </si>
   <si>
     <t>conjugated_cat_number</t>
@@ -556,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -565,7 +529,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,24 +557,11 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="H2:H1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ug/ml." sqref="I2:I1048576">
-      <formula1>'concentration_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -634,22 +585,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>